<commit_message>
Modificate ore in redazione relazione finale
</commit_message>
<xml_diff>
--- a/SuddivsioneAttività.xlsx
+++ b/SuddivsioneAttività.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristian/Documents/MATLAB/Embedded/PW MRC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C269DF9-84AD-4454-9E62-A54586F88F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DEF965-1FC2-4540-B763-9559DEC7930A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{C1632790-AC48-46BD-AD2C-80684938B368}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{C1632790-AC48-46BD-AD2C-80684938B368}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -174,7 +174,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -492,24 +491,24 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="65.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -520,52 +519,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -576,52 +570,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11">
         <v>8</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -632,52 +621,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15">
         <v>10</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16">
         <v>10</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17">
         <v>10</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -688,52 +672,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21">
         <v>3</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22">
         <v>3</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23">
         <v>3</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>3</v>
       </c>
@@ -744,36 +723,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="4">
-        <v>2</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="4">
-        <v>2</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="4">
-        <v>2</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>